<commit_message>
1. remove outdated interfaces
2. weighted configuration selection
</commit_message>
<xml_diff>
--- a/classifier/result.xlsx
+++ b/classifier/result.xlsx
@@ -22,7 +22,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">job_id</t>
+  </si>
   <si>
     <t xml:space="preserve">m1.medium 4</t>
   </si>
@@ -127,11 +130,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,132 +155,137 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9878542510121"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8825910931174"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2348178137652"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>73.78</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="0" t="n">
         <v>56.01</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="0" t="n">
         <v>62.92</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="0" t="n">
         <v>52.22</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="0" t="n">
         <v>56.75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>36.43</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="0" t="n">
         <v>22.59</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="0" t="n">
         <v>31.18</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="0" t="n">
         <v>27.38</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="0" t="n">
         <v>30.13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>162.43</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="0" t="n">
         <v>159.71</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="0" t="n">
         <v>106.17</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="0" t="n">
         <v>115.73</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="0" t="n">
         <v>85.68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>342.33</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="0" t="n">
         <v>381.85</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="0" t="n">
         <v>358.34</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="0" t="n">
         <v>380.36</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="0" t="n">
         <v>363.41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="n">
         <v>548.92</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="0" t="n">
         <v>278.22</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="0" t="n">
         <v>365.9</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="0" t="n">
         <v>283.04</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="0" t="n">
         <v>289.98</v>
       </c>
     </row>
@@ -308,6 +312,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -331,6 +338,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>